<commit_message>
finished ciena doc builder
</commit_message>
<xml_diff>
--- a/Ciena/CATP_Master_Feature_List.xlsx
+++ b/Ciena/CATP_Master_Feature_List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mzheng\Coding\Python\ixia_automation\Ciena\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E22E1AFF-255D-455B-92E3-94044B2592AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA35E9E1-22F6-4051-A7DD-029A74978BC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1080" yWindow="300" windowWidth="19460" windowHeight="8650" xr2:uid="{DF307320-4771-4B2E-8F0B-9CA3C6235913}"/>
+    <workbookView xWindow="-350" yWindow="440" windowWidth="19200" windowHeight="8650" xr2:uid="{DF307320-4771-4B2E-8F0B-9CA3C6235913}"/>
   </bookViews>
   <sheets>
     <sheet name="CATP Input" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="278">
   <si>
     <t>All installs require</t>
   </si>
@@ -114,18 +114,12 @@
     <t>2.2.16 Syslog over TLS configuration</t>
   </si>
   <si>
-    <t>2.2.17 SSH Public Key Authentication</t>
-  </si>
-  <si>
     <t>2.2.18 SSH Rekeying Configuration</t>
   </si>
   <si>
     <t>2.2.19 DNS Client Setup</t>
   </si>
   <si>
-    <t>2.2.20 L3 DHCPv4 Relay Setup</t>
-  </si>
-  <si>
     <t>2.2.21 DHCPv6 Client Setup</t>
   </si>
   <si>
@@ -868,6 +862,15 @@
   </si>
   <si>
     <t>******Beginning of CATP Part II******</t>
+  </si>
+  <si>
+    <t>5.11.4              Configurable BFD session Parameters</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>5.23.1       IGMP snooping Config</t>
   </si>
 </sst>
 </file>
@@ -883,7 +886,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -893,6 +896,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -909,9 +918,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1226,10 +1236,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFD19FB1-FD87-4C3C-87AC-AD521B537A47}">
-  <dimension ref="B2:F260"/>
+  <dimension ref="B2:F251"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="F165" sqref="F165"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="F249" sqref="F249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1244,13 +1254,13 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.35">
@@ -1258,7 +1268,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
@@ -1269,7 +1279,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -1280,7 +1290,7 @@
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
@@ -1291,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -1302,7 +1312,7 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
         <v>11</v>
@@ -1313,7 +1323,7 @@
         <v>16</v>
       </c>
       <c r="D8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -1324,13 +1334,13 @@
         <v>18</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.35">
@@ -1338,27 +1348,27 @@
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s">
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.35">
@@ -1366,7 +1376,7 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.35">
@@ -1409,22 +1419,22 @@
         <v>27</v>
       </c>
       <c r="F20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E21" s="1" t="s">
+      <c r="E21" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="22" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="5:6" x14ac:dyDescent="0.35">
@@ -1483,21 +1493,21 @@
       </c>
     </row>
     <row r="35" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E35" t="s">
-        <v>43</v>
+      <c r="E35" s="1" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="36" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E36" t="s">
+        <v>45</v>
+      </c>
+      <c r="F36" t="s">
         <v>44</v>
       </c>
-      <c r="F36" t="s">
+    </row>
+    <row r="37" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E37" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="E37" s="1" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="38" spans="5:6" x14ac:dyDescent="0.35">
@@ -1505,7 +1515,7 @@
         <v>47</v>
       </c>
       <c r="F38" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="39" spans="5:6" x14ac:dyDescent="0.35">
@@ -1513,7 +1523,7 @@
         <v>48</v>
       </c>
       <c r="F39" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="40" spans="5:6" x14ac:dyDescent="0.35">
@@ -1521,7 +1531,7 @@
         <v>49</v>
       </c>
       <c r="F40" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="41" spans="5:6" x14ac:dyDescent="0.35">
@@ -1529,7 +1539,7 @@
         <v>50</v>
       </c>
       <c r="F41" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="42" spans="5:6" x14ac:dyDescent="0.35">
@@ -1643,7 +1653,7 @@
       </c>
     </row>
     <row r="64" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E64" t="s">
+      <c r="E64" s="1" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1658,7 +1668,7 @@
       </c>
     </row>
     <row r="67" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E67" t="s">
+      <c r="E67" s="1" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1668,7 +1678,7 @@
       </c>
     </row>
     <row r="69" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E69" s="1" t="s">
+      <c r="E69" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1799,330 +1809,354 @@
     </row>
     <row r="95" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E95" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="96" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E96" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="97" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E97" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="98" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E98" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="F98" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="99" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E99" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="100" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E100" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="101" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E101" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E100" t="s">
+    <row r="102" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E102" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E101" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E102" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E103" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="104" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E104" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="105" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E105" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E106" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="107" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E107" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="108" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E108" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="109" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E109" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E110" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E111" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E112" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="113" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E113" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="114" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E114" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="F114" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="115" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E115" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="116" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E116" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="117" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E117" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="118" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E118" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="119" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E119" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="120" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E120" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="121" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E121" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="122" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E122" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="123" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E123" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="124" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E124" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="125" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E125" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="126" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E126" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="127" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E127" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="128" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E128" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="129" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E129" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="130" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E130" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="F130" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="131" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E131" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="132" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E132" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="133" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E133" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="F133" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="134" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E134" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="135" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E135" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="136" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E136" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="137" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E137" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="138" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E138" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="139" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E139" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E139" t="s">
+    <row r="140" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E140" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E140" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="F140" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="141" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E141" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="142" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E142" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="143" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E143" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E144" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E145" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="146" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E146" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="147" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E147" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E148" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E149" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="F149" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="150" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E150" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E151" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E152" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="F152" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="153" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E153" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="154" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E154" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="155" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E155" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="156" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E156" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="157" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="F156" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="157" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E157" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="158" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E158" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="159" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E159" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="160" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E160" t="s">
         <v>167</v>
       </c>
@@ -2136,29 +2170,32 @@
       <c r="E162" t="s">
         <v>169</v>
       </c>
+      <c r="F162" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="163" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E163" t="s">
-        <v>170</v>
+        <v>226</v>
       </c>
     </row>
     <row r="164" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E164" t="s">
-        <v>171</v>
+        <v>227</v>
       </c>
     </row>
     <row r="165" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E165" t="s">
         <v>228</v>
       </c>
-      <c r="F165" t="s">
-        <v>46</v>
-      </c>
     </row>
     <row r="166" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E166" t="s">
         <v>229</v>
       </c>
+      <c r="F166" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="167" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E167" t="s">
@@ -2177,28 +2214,34 @@
     </row>
     <row r="170" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E170" t="s">
-        <v>172</v>
+        <v>233</v>
       </c>
     </row>
     <row r="171" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E171" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="172" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E172" t="s">
-        <v>234</v>
+        <v>235</v>
+      </c>
+      <c r="F172" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="173" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E173" t="s">
-        <v>235</v>
+        <v>171</v>
       </c>
     </row>
     <row r="174" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E174" t="s">
         <v>236</v>
       </c>
+      <c r="F174" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="175" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E175" t="s">
@@ -2207,427 +2250,400 @@
     </row>
     <row r="176" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E176" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="177" spans="5:5" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="177" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E177" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="178" spans="5:5" x14ac:dyDescent="0.35">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="178" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E178" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="179" spans="5:5" x14ac:dyDescent="0.35">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="179" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E179" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E180" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="181" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E181" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="182" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E182" t="s">
+        <v>243</v>
+      </c>
+      <c r="F182" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="183" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E183" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="184" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E184" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="185" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E185" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="186" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E186" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="187" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E187" t="s">
+        <v>248</v>
+      </c>
+      <c r="F187" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="188" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E188" s="2" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E182" t="s">
+    <row r="189" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E189" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E183" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E184" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E185" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E186" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="187" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E187" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="188" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E188" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="189" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E189" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="190" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="190" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E190" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="191" spans="5:5" x14ac:dyDescent="0.35">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="191" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E191" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="192" spans="5:5" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="192" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E192" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="193" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E193" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
     <row r="194" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E194" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="195" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E195" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="196" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E196" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
     </row>
     <row r="197" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E197" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="198" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E198" t="s">
-        <v>182</v>
+        <v>249</v>
       </c>
     </row>
     <row r="199" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E199" t="s">
-        <v>183</v>
+        <v>250</v>
       </c>
     </row>
     <row r="200" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E200" t="s">
-        <v>184</v>
+        <v>251</v>
       </c>
     </row>
     <row r="201" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E201" t="s">
-        <v>185</v>
+        <v>252</v>
       </c>
     </row>
     <row r="202" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E202" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
     </row>
     <row r="203" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E203" t="s">
-        <v>252</v>
+        <v>184</v>
       </c>
     </row>
     <row r="204" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E204" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
     </row>
     <row r="205" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E205" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="206" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E206" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="207" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E207" t="s">
-        <v>186</v>
+        <v>257</v>
       </c>
     </row>
     <row r="208" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E208" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
     </row>
     <row r="209" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E209" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="210" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E210" t="s">
-        <v>258</v>
+        <v>185</v>
       </c>
     </row>
     <row r="211" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E211" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="212" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E212" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="213" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E213" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="214" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E214" t="s">
-        <v>187</v>
+        <v>263</v>
       </c>
     </row>
     <row r="215" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E215" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
     </row>
     <row r="216" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E216" t="s">
-        <v>263</v>
+        <v>186</v>
       </c>
     </row>
     <row r="217" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E217" t="s">
-        <v>264</v>
+        <v>187</v>
       </c>
     </row>
     <row r="218" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E218" t="s">
-        <v>265</v>
+        <v>188</v>
       </c>
     </row>
     <row r="219" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E219" t="s">
-        <v>266</v>
+        <v>189</v>
       </c>
     </row>
     <row r="220" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E220" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="221" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E221" t="s">
-        <v>189</v>
+        <v>265</v>
       </c>
     </row>
     <row r="222" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E222" t="s">
-        <v>190</v>
+        <v>266</v>
       </c>
     </row>
     <row r="223" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E223" t="s">
-        <v>191</v>
+        <v>267</v>
       </c>
     </row>
     <row r="224" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E224" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="225" spans="5:5" x14ac:dyDescent="0.35">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="225" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E225" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="226" spans="5:5" x14ac:dyDescent="0.35">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="226" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E226" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="227" spans="5:5" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="227" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E227" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="228" spans="5:5" x14ac:dyDescent="0.35">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="228" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E228" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="229" spans="5:5" x14ac:dyDescent="0.35">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="229" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E229" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="230" spans="5:5" x14ac:dyDescent="0.35">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="230" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E230" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="231" spans="5:5" x14ac:dyDescent="0.35">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="231" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E231" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="232" spans="5:5" x14ac:dyDescent="0.35">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="232" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E232" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="233" spans="5:5" x14ac:dyDescent="0.35">
+        <v>199</v>
+      </c>
+      <c r="F232" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="233" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E233" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="234" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E234" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="235" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E235" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="236" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E236" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="237" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E237" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="238" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E238" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="239" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E239" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="240" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E240" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="241" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E241" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="242" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E242" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="243" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E243" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="244" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E244" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="245" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E245" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="246" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E246" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="247" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E247" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="248" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E248" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="249" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E249" t="s">
+        <v>216</v>
+      </c>
+      <c r="F249" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="250" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E250" t="s">
+        <v>217</v>
+      </c>
+      <c r="F250" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="251" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E251" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="234" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E234" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="235" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E235" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="236" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E236" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="237" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E237" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="238" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E238" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="239" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E239" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="240" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E240" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="241" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E241" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="242" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E242" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="243" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E243" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="244" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E244" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="245" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E245" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="246" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E246" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="247" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E247" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="248" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E248" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="249" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E249" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="250" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E250" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="251" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E251" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="252" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E252" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="253" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E253" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="254" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E254" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="255" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E255" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="256" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E256" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="257" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E257" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="258" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E258" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="259" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E259" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="260" spans="5:5" x14ac:dyDescent="0.35">
-      <c r="E260" t="s">
-        <v>275</v>
+      <c r="F251" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -2651,7 +2667,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B1">
         <v>21</v>
@@ -2659,7 +2675,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2">
         <v>21</v>
@@ -2667,7 +2683,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3">
         <v>23</v>
@@ -2675,7 +2691,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B4">
         <v>25</v>
@@ -2683,7 +2699,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B5">
         <v>26</v>
@@ -2691,7 +2707,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B6">
         <v>28</v>
@@ -2699,7 +2715,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B7">
         <v>31</v>
@@ -2707,7 +2723,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B8">
         <v>32</v>
@@ -2715,7 +2731,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9">
         <v>34</v>
@@ -2723,7 +2739,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B10">
         <v>36</v>
@@ -2731,7 +2747,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B11">
         <v>37</v>
@@ -2739,7 +2755,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B12">
         <v>39</v>
@@ -2747,7 +2763,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B13">
         <v>40</v>
@@ -2755,7 +2771,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B14">
         <v>41</v>
@@ -2763,7 +2779,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B15">
         <v>42</v>
@@ -2771,7 +2787,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B16">
         <v>43</v>
@@ -2779,7 +2795,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B17">
         <v>45</v>
@@ -2787,7 +2803,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B18">
         <v>46</v>
@@ -2795,7 +2811,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B19">
         <v>48</v>
@@ -2803,7 +2819,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B20">
         <v>49</v>
@@ -2811,7 +2827,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B21">
         <v>51</v>
@@ -2819,7 +2835,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B22">
         <v>53</v>
@@ -2827,7 +2843,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B23">
         <v>53</v>
@@ -2835,7 +2851,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B24">
         <v>55</v>
@@ -2843,7 +2859,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B25">
         <v>56</v>
@@ -2851,7 +2867,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B26">
         <v>58</v>
@@ -2859,7 +2875,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B27">
         <v>59</v>
@@ -2867,7 +2883,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B28">
         <v>61</v>
@@ -2875,7 +2891,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B29">
         <v>64</v>
@@ -2883,7 +2899,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B30">
         <v>65</v>
@@ -2891,7 +2907,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B31">
         <v>67</v>
@@ -2899,7 +2915,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B32">
         <v>68</v>
@@ -2907,7 +2923,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B33">
         <v>69</v>
@@ -2915,7 +2931,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B34">
         <v>70</v>
@@ -2923,7 +2939,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B35">
         <v>73</v>
@@ -2931,7 +2947,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B36">
         <v>75</v>
@@ -2939,7 +2955,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B37">
         <v>77</v>
@@ -2947,7 +2963,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B38">
         <v>79</v>
@@ -2955,7 +2971,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B39">
         <v>79</v>
@@ -2963,7 +2979,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B40">
         <v>80</v>
@@ -2971,7 +2987,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B41">
         <v>82</v>
@@ -2979,7 +2995,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B42">
         <v>82</v>
@@ -2987,7 +3003,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B43">
         <v>84</v>
@@ -2995,7 +3011,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B44">
         <v>85</v>
@@ -3003,7 +3019,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B45">
         <v>86</v>
@@ -3011,7 +3027,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B46">
         <v>88</v>
@@ -3019,7 +3035,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B47">
         <v>90</v>
@@ -3027,7 +3043,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B48">
         <v>92</v>
@@ -3035,7 +3051,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B49">
         <v>93</v>
@@ -3043,7 +3059,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B50">
         <v>99</v>
@@ -3051,7 +3067,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B51">
         <v>101</v>
@@ -3059,7 +3075,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B52">
         <v>105</v>
@@ -3067,7 +3083,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B53">
         <v>107</v>
@@ -3075,7 +3091,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B54">
         <v>107</v>
@@ -3083,7 +3099,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B55">
         <v>109</v>
@@ -3091,7 +3107,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B56">
         <v>110</v>
@@ -3099,7 +3115,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B57">
         <v>113</v>
@@ -3107,7 +3123,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B58">
         <v>113</v>
@@ -3115,7 +3131,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B59">
         <v>117</v>
@@ -3123,7 +3139,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B60">
         <v>118</v>
@@ -3131,7 +3147,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B61">
         <v>119</v>
@@ -3139,7 +3155,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B62">
         <v>120</v>
@@ -3147,7 +3163,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B63">
         <v>124</v>
@@ -3155,7 +3171,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B64">
         <v>124</v>
@@ -3163,7 +3179,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B65">
         <v>127</v>
@@ -3171,7 +3187,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B66">
         <v>130</v>
@@ -3179,7 +3195,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B67">
         <v>131</v>
@@ -3187,7 +3203,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B68">
         <v>133</v>
@@ -3195,7 +3211,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B69">
         <v>134</v>
@@ -3203,7 +3219,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B70">
         <v>135</v>
@@ -3211,7 +3227,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B71">
         <v>139</v>
@@ -3219,7 +3235,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B72">
         <v>142</v>
@@ -3227,7 +3243,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B73">
         <v>143</v>
@@ -3235,7 +3251,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B74">
         <v>144</v>
@@ -3243,7 +3259,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B75">
         <v>147</v>
@@ -3251,7 +3267,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B76">
         <v>148</v>
@@ -3259,7 +3275,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B77">
         <v>151</v>
@@ -3267,7 +3283,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B78">
         <v>152</v>
@@ -3275,7 +3291,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B79">
         <v>153</v>
@@ -3283,7 +3299,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B80">
         <v>154</v>
@@ -3291,7 +3307,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B81">
         <v>156</v>
@@ -3299,7 +3315,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B82">
         <v>158</v>
@@ -3307,7 +3323,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B83">
         <v>160</v>
@@ -3315,7 +3331,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B84">
         <v>162</v>
@@ -3323,7 +3339,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B85">
         <v>163</v>
@@ -3331,7 +3347,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B86">
         <v>165</v>
@@ -3339,7 +3355,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B87">
         <v>168</v>
@@ -3347,7 +3363,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B88">
         <v>169</v>
@@ -3355,7 +3371,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B89">
         <v>184</v>
@@ -3363,7 +3379,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B90">
         <v>199</v>
@@ -3371,7 +3387,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B91">
         <v>201</v>
@@ -3379,7 +3395,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B92">
         <v>217</v>
@@ -3387,7 +3403,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B93">
         <v>220</v>
@@ -3395,7 +3411,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B94">
         <v>227</v>
@@ -3403,7 +3419,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B95">
         <v>230</v>
@@ -3411,7 +3427,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B96">
         <v>233</v>
@@ -3419,7 +3435,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B97">
         <v>235</v>
@@ -3427,7 +3443,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B98">
         <v>236</v>
@@ -3435,7 +3451,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B99">
         <v>243</v>
@@ -3443,7 +3459,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B100">
         <v>249</v>
@@ -3451,7 +3467,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B101">
         <v>251</v>
@@ -3459,7 +3475,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B102">
         <v>252</v>
@@ -3467,7 +3483,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B103">
         <v>253</v>
@@ -3475,7 +3491,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B104">
         <v>254</v>
@@ -3483,7 +3499,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B105">
         <v>256</v>
@@ -3491,7 +3507,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B106">
         <v>258</v>
@@ -3499,7 +3515,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B107">
         <v>262</v>
@@ -3507,7 +3523,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B108">
         <v>264</v>
@@ -3515,7 +3531,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B109">
         <v>265</v>
@@ -3523,7 +3539,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B110">
         <v>266</v>
@@ -3531,7 +3547,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B111">
         <v>268</v>
@@ -3539,7 +3555,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B112">
         <v>274</v>
@@ -3547,7 +3563,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B113">
         <v>276</v>
@@ -3555,7 +3571,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B114">
         <v>278</v>
@@ -3563,7 +3579,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B115">
         <v>280</v>
@@ -3571,7 +3587,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B116">
         <v>281</v>
@@ -3579,7 +3595,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B117">
         <v>282</v>
@@ -3587,7 +3603,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B118">
         <v>285</v>
@@ -3595,7 +3611,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B119">
         <v>287</v>
@@ -3603,7 +3619,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B120">
         <v>288</v>
@@ -3611,7 +3627,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B121">
         <v>291</v>
@@ -3619,7 +3635,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B122">
         <v>294</v>
@@ -3627,7 +3643,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B123">
         <v>294</v>
@@ -3635,7 +3651,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B124">
         <v>306</v>
@@ -3643,7 +3659,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B125">
         <v>311</v>
@@ -3651,7 +3667,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B126">
         <v>312</v>
@@ -3659,7 +3675,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B127">
         <v>316</v>
@@ -3667,7 +3683,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B128">
         <v>321</v>
@@ -3675,7 +3691,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B129">
         <v>324</v>
@@ -3683,7 +3699,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B130">
         <v>326</v>
@@ -3691,7 +3707,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B131">
         <v>332</v>
@@ -3699,7 +3715,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B132">
         <v>334</v>
@@ -3707,7 +3723,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B133">
         <v>338</v>
@@ -3715,7 +3731,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B134">
         <v>346</v>
@@ -3723,7 +3739,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B135">
         <v>349</v>
@@ -3731,7 +3747,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B136">
         <v>351</v>
@@ -3739,7 +3755,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B137">
         <v>353</v>
@@ -3747,7 +3763,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B138">
         <v>355</v>
@@ -3755,7 +3771,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B139">
         <v>356</v>
@@ -3763,7 +3779,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B140">
         <v>357</v>
@@ -3771,7 +3787,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B141">
         <v>359</v>
@@ -3779,7 +3795,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B142">
         <v>360</v>
@@ -3787,7 +3803,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B143">
         <v>362</v>
@@ -3795,7 +3811,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B144">
         <v>363</v>
@@ -3803,7 +3819,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B145">
         <v>363</v>
@@ -3811,7 +3827,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B146">
         <v>364</v>
@@ -3819,7 +3835,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B147">
         <v>366</v>
@@ -3827,7 +3843,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B148">
         <v>367</v>
@@ -3835,7 +3851,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B149">
         <v>368</v>
@@ -3843,7 +3859,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B150">
         <v>369</v>
@@ -3851,7 +3867,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B151">
         <v>374</v>
@@ -3859,7 +3875,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B152">
         <v>375</v>
@@ -3867,7 +3883,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B153">
         <v>378</v>
@@ -3875,7 +3891,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B154">
         <v>381</v>
@@ -3883,7 +3899,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B155">
         <v>383</v>
@@ -3891,7 +3907,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B156">
         <v>385</v>
@@ -3899,7 +3915,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B157">
         <v>386</v>
@@ -3907,7 +3923,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B158">
         <v>389</v>
@@ -3915,7 +3931,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B159">
         <v>390</v>
@@ -3923,7 +3939,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B160">
         <v>390</v>
@@ -3931,7 +3947,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B161">
         <v>391</v>
@@ -3939,7 +3955,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B162">
         <v>400</v>
@@ -3947,7 +3963,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B163">
         <v>405</v>
@@ -3955,7 +3971,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B164">
         <v>408</v>
@@ -3963,7 +3979,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B165">
         <v>408</v>
@@ -3971,7 +3987,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B166">
         <v>409</v>
@@ -3979,7 +3995,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B167">
         <v>411</v>
@@ -3987,7 +4003,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B168">
         <v>415</v>
@@ -3995,7 +4011,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B169">
         <v>415</v>
@@ -4003,7 +4019,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B170">
         <v>428</v>
@@ -4011,7 +4027,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B171">
         <v>429</v>
@@ -4019,7 +4035,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B172">
         <v>431</v>
@@ -4027,7 +4043,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B173">
         <v>432</v>
@@ -4035,7 +4051,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B174">
         <v>433</v>
@@ -4043,7 +4059,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B175">
         <v>434</v>
@@ -4051,7 +4067,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B176">
         <v>438</v>
@@ -4059,7 +4075,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B177">
         <v>439</v>
@@ -4067,7 +4083,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B178">
         <v>441</v>
@@ -4075,7 +4091,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B179">
         <v>442</v>
@@ -4083,7 +4099,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B180">
         <v>443</v>
@@ -4091,7 +4107,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B181">
         <v>444</v>
@@ -4099,7 +4115,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B182">
         <v>445</v>
@@ -4107,7 +4123,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B183">
         <v>445</v>
@@ -4115,7 +4131,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B184">
         <v>446</v>
@@ -4123,7 +4139,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B185">
         <v>448</v>
@@ -4131,7 +4147,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B186">
         <v>449</v>
@@ -4139,7 +4155,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B187">
         <v>450</v>
@@ -4147,7 +4163,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B188">
         <v>451</v>
@@ -4155,7 +4171,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B189">
         <v>454</v>
@@ -4163,7 +4179,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B190">
         <v>456</v>
@@ -4171,7 +4187,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B191">
         <v>458</v>
@@ -4179,7 +4195,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B192">
         <v>458</v>
@@ -4187,7 +4203,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B193">
         <v>459</v>
@@ -4195,7 +4211,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B194">
         <v>459</v>
@@ -4203,7 +4219,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B195">
         <v>460</v>
@@ -4211,7 +4227,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B196">
         <v>460</v>
@@ -4219,7 +4235,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B197">
         <v>461</v>
@@ -4227,7 +4243,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B198">
         <v>461</v>
@@ -4235,7 +4251,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B199">
         <v>461</v>
@@ -4243,7 +4259,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B200">
         <v>462</v>
@@ -4251,7 +4267,7 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B201">
         <v>463</v>
@@ -4259,7 +4275,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B202">
         <v>465</v>
@@ -4267,7 +4283,7 @@
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B203">
         <v>468</v>
@@ -4275,7 +4291,7 @@
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B204">
         <v>470</v>
@@ -4283,7 +4299,7 @@
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B205">
         <v>470</v>
@@ -4291,7 +4307,7 @@
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B206">
         <v>472</v>
@@ -4299,7 +4315,7 @@
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B207">
         <v>474</v>
@@ -4307,7 +4323,7 @@
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B208">
         <v>475</v>
@@ -4315,7 +4331,7 @@
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B209">
         <v>477</v>
@@ -4323,7 +4339,7 @@
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B210">
         <v>478</v>
@@ -4331,7 +4347,7 @@
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B211">
         <v>479</v>
@@ -4339,7 +4355,7 @@
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B212">
         <v>480</v>
@@ -4347,7 +4363,7 @@
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B213">
         <v>480</v>
@@ -4355,7 +4371,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B214">
         <v>481</v>
@@ -4363,7 +4379,7 @@
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B215">
         <v>482</v>
@@ -4371,7 +4387,7 @@
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B216">
         <v>483</v>
@@ -4379,7 +4395,7 @@
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B217">
         <v>485</v>
@@ -4387,7 +4403,7 @@
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B218">
         <v>486</v>
@@ -4395,7 +4411,7 @@
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B219">
         <v>487</v>
@@ -4403,7 +4419,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B220">
         <v>491</v>
@@ -4411,7 +4427,7 @@
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B221">
         <v>491</v>
@@ -4419,7 +4435,7 @@
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B222">
         <v>500</v>
@@ -4427,7 +4443,7 @@
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B223">
         <v>509</v>
@@ -4435,7 +4451,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B224">
         <v>512</v>
@@ -4443,7 +4459,7 @@
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B225">
         <v>516</v>
@@ -4451,7 +4467,7 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B226">
         <v>518</v>
@@ -4459,7 +4475,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B227">
         <v>521</v>
@@ -4467,7 +4483,7 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B228">
         <v>524</v>
@@ -4475,7 +4491,7 @@
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B229">
         <v>528</v>

</xml_diff>